<commit_message>
added reading of version and sbol3 update for multi instance
</commit_message>
<xml_diff>
--- a/excel2sbol/tests/test_files/pichia_comb_dev_compiler_sbol3_v006.xlsx
+++ b/excel2sbol/tests/test_files/pichia_comb_dev_compiler_sbol3_v006.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7782" uniqueCount="7593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7791" uniqueCount="7597">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22816,29 +22816,6 @@
     <t>"http:\/\/identifiers.org/so/SO:[0-9]" "http:\/\/purl.obolibrary.org/obo/SO_[0-9]{7}"</t>
   </si>
   <si>
-    <r>
-      <t>"^[a-zA-Z \s*]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>$" "https:\/\/www.ncbi.nlm.nih.gov/nuccore/.*"</t>
-    </r>
-  </si>
-  <si>
     <t>sbol_types</t>
   </si>
   <si>
@@ -22852,13 +22829,28 @@
   </si>
   <si>
     <t>Init</t>
+  </si>
+  <si>
+    <t>SBOL Version</t>
+  </si>
+  <si>
+    <t>ATTTGC</t>
+  </si>
+  <si>
+    <t>https://www.pnas.org/content/pnas/95/17/9761.full.pdf</t>
+  </si>
+  <si>
+    <t>ATP07149.1</t>
+  </si>
+  <si>
+    <t>E0040</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -23030,14 +23022,20 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFD4D4D4"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -23157,12 +23155,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -23219,75 +23219,18 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="74">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -23339,6 +23282,33 @@
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
         <horizontal/>
       </border>
     </dxf>
@@ -24071,6 +24041,86 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -24111,12 +24161,157 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="1">
+  <tableStyles count="6">
     <tableStyle name="Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="55"/>
-      <tableStyleElement type="firstRowStripe" dxfId="54"/>
-      <tableStyleElement type="secondRowStripe" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="73"/>
+      <tableStyleElement type="firstRowStripe" dxfId="72"/>
+      <tableStyleElement type="secondRowStripe" dxfId="71"/>
+    </tableStyle>
+    <tableStyle name="Basic Parts-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="70"/>
+      <tableStyleElement type="firstRowStripe" dxfId="69"/>
+      <tableStyleElement type="secondRowStripe" dxfId="68"/>
+    </tableStyle>
+    <tableStyle name="Composite Parts-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="67"/>
+      <tableStyleElement type="firstRowStripe" dxfId="66"/>
+      <tableStyleElement type="secondRowStripe" dxfId="65"/>
+    </tableStyle>
+    <tableStyle name="Composite Parts-style 2" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="64"/>
+      <tableStyleElement type="firstRowStripe" dxfId="63"/>
+      <tableStyleElement type="secondRowStripe" dxfId="62"/>
+    </tableStyle>
+    <tableStyle name="Composite Parts-style 3" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="61"/>
+      <tableStyleElement type="firstRowStripe" dxfId="60"/>
+      <tableStyleElement type="secondRowStripe" dxfId="59"/>
+    </tableStyle>
+    <tableStyle name="Composite Parts-style 4" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="58"/>
+      <tableStyleElement type="firstRowStripe" dxfId="57"/>
+      <tableStyleElement type="secondRowStripe" dxfId="56"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -24128,7 +24323,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A10:J16" totalsRowShown="0" headerRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A10:J16" totalsRowShown="0" headerRowDxfId="55">
   <autoFilter ref="A10:J16"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Sheet Name"/>
@@ -24147,57 +24342,58 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P19" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P19" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:P19"/>
   <tableColumns count="16">
-    <tableColumn id="16" name="Sheet Name" dataDxfId="49"/>
-    <tableColumn id="1" name="Column Name" dataDxfId="48"/>
-    <tableColumn id="2" name="SBOL Term" dataDxfId="47"/>
-    <tableColumn id="3" name="Namespace URL" dataDxfId="46"/>
-    <tableColumn id="17" name="Type" dataDxfId="45" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Split On" dataDxfId="44"/>
-    <tableColumn id="6" name="Pattern" dataDxfId="43"/>
-    <tableColumn id="7" name="Tyto Lookup" dataDxfId="42"/>
-    <tableColumn id="8" name="Sheet Lookup" dataDxfId="41"/>
-    <tableColumn id="9" name="Replacement Lookup" dataDxfId="40"/>
-    <tableColumn id="10" name="Object_ID Lookup" dataDxfId="39"/>
-    <tableColumn id="11" name="Parent Lookup" dataDxfId="38"/>
-    <tableColumn id="12" name="Lookup Sheet Name" dataDxfId="37"/>
-    <tableColumn id="13" name="From Col" dataDxfId="36"/>
-    <tableColumn id="14" name="To Col" dataDxfId="35"/>
-    <tableColumn id="15" name="Ontology Name" dataDxfId="34"/>
+    <tableColumn id="16" name="Sheet Name" dataDxfId="44"/>
+    <tableColumn id="1" name="Column Name" dataDxfId="43"/>
+    <tableColumn id="2" name="SBOL Term" dataDxfId="42"/>
+    <tableColumn id="3" name="Namespace URL" dataDxfId="41"/>
+    <tableColumn id="17" name="Type" dataDxfId="40" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="Split On" dataDxfId="39"/>
+    <tableColumn id="6" name="Pattern" dataDxfId="38"/>
+    <tableColumn id="7" name="Tyto Lookup" dataDxfId="37"/>
+    <tableColumn id="8" name="Sheet Lookup" dataDxfId="36"/>
+    <tableColumn id="9" name="Replacement Lookup" dataDxfId="35"/>
+    <tableColumn id="10" name="Object_ID Lookup" dataDxfId="34"/>
+    <tableColumn id="11" name="Parent Lookup" dataDxfId="33"/>
+    <tableColumn id="12" name="Lookup Sheet Name" dataDxfId="32"/>
+    <tableColumn id="13" name="From Col" dataDxfId="31"/>
+    <tableColumn id="14" name="To Col" dataDxfId="30"/>
+    <tableColumn id="15" name="Ontology Name" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table_14" displayName="Table_14" ref="A5:C7" headerRowDxfId="33" totalsRowDxfId="30" headerRowBorderDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table_14" displayName="Table_14" ref="A5:C7" headerRowDxfId="28" totalsRowDxfId="25" headerRowBorderDxfId="27" tableBorderDxfId="26">
   <tableColumns count="3">
-    <tableColumn id="1" name="Collection Name" dataDxfId="29"/>
-    <tableColumn id="16" name="SBOL Object Type" dataDxfId="28"/>
-    <tableColumn id="5" name="Description" dataDxfId="27"/>
+    <tableColumn id="1" name="Collection Name" dataDxfId="24"/>
+    <tableColumn id="16" name="SBOL Object Type" dataDxfId="23"/>
+    <tableColumn id="5" name="Description" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="Library-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A4:M12" headerRowDxfId="26" totalsRowDxfId="23" headerRowBorderDxfId="25" tableBorderDxfId="24">
-  <tableColumns count="13">
-    <tableColumn id="1" name="Part Name" dataDxfId="22"/>
-    <tableColumn id="11" name="Collection" dataDxfId="21"/>
-    <tableColumn id="12" name="Molecule Type" dataDxfId="20"/>
-    <tableColumn id="2" name="Role" dataDxfId="19"/>
-    <tableColumn id="3" name="Alteration 1" dataDxfId="18"/>
-    <tableColumn id="15" name="Alteration" dataDxfId="17"/>
-    <tableColumn id="5" name="Part Description" dataDxfId="16"/>
-    <tableColumn id="4" name="More info" dataDxfId="15"/>
-    <tableColumn id="6" name="Data Source Prefix" dataDxfId="14"/>
-    <tableColumn id="7" name="Data Source" dataDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="Source Organism" dataDxfId="12"/>
-    <tableColumn id="10" name="Circular" dataDxfId="11"/>
-    <tableColumn id="13" name="Data Source Composite" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A4:N12" headerRowDxfId="21" totalsRowDxfId="18" headerRowBorderDxfId="20" tableBorderDxfId="19">
+  <tableColumns count="14">
+    <tableColumn id="1" name="Part Name" dataDxfId="17"/>
+    <tableColumn id="11" name="Collection" dataDxfId="16"/>
+    <tableColumn id="12" name="Molecule Type" dataDxfId="15"/>
+    <tableColumn id="2" name="Role" dataDxfId="14"/>
+    <tableColumn id="3" name="Alteration 1" dataDxfId="13"/>
+    <tableColumn id="15" name="Alteration" dataDxfId="12"/>
+    <tableColumn id="5" name="Part Description" dataDxfId="11"/>
+    <tableColumn id="4" name="More info" dataDxfId="10"/>
+    <tableColumn id="6" name="Data Source Prefix" dataDxfId="9"/>
+    <tableColumn id="7" name="Data Source" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="Source Organism" dataDxfId="7"/>
+    <tableColumn id="10" name="Circular" dataDxfId="6"/>
+    <tableColumn id="9" name="Sequence" dataDxfId="5"/>
+    <tableColumn id="13" name="Data Source Composite" dataDxfId="4">
       <calculatedColumnFormula>Library!$I5&amp;":"&amp;Library!$J5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24409,7 +24605,7 @@
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -24426,18 +24622,26 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
-        <v>7534</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>7555</v>
+        <v>7592</v>
+      </c>
+      <c r="B1" s="27">
+        <v>3</v>
       </c>
       <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
+        <v>7534</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>7555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
         <v>7535</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
     </row>
@@ -24490,7 +24694,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>7491</v>
+        <v>7489</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -25812,7 +26016,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -25974,7 +26178,7 @@
         <v>7556</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>7588</v>
+        <v>7587</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>7554</v>
@@ -26334,10 +26538,10 @@
         <v>7537</v>
       </c>
       <c r="B12" s="54" t="s">
+        <v>7589</v>
+      </c>
+      <c r="C12" s="49" t="s">
         <v>7590</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>7591</v>
       </c>
       <c r="D12" s="49" t="s">
         <v>7554</v>
@@ -26374,13 +26578,13 @@
         <v>7537</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>7589</v>
+        <v>7588</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>7591</v>
-      </c>
-      <c r="D13" s="49" t="s">
-        <v>7554</v>
+        <v>7585</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>7433</v>
       </c>
       <c r="E13" s="51" t="s">
         <v>7450</v>
@@ -26428,9 +26632,7 @@
       <c r="F14" s="51" t="s">
         <v>7452</v>
       </c>
-      <c r="G14" s="51" t="s">
-        <v>7587</v>
-      </c>
+      <c r="G14" s="51"/>
       <c r="H14" s="49" t="b">
         <v>0</v>
       </c>
@@ -26619,7 +26821,7 @@
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="55" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>7488</v>
@@ -26695,34 +26897,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H14:L18 H2:L11">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="12" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:L12">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="10" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:L19">
+    <cfRule type="cellIs" dxfId="48" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:L13">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19:L19">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26734,11 +26936,12 @@
     <hyperlink ref="D15" r:id="rId5" display="https://wiki.synbiohub.org/wiki/Terms/synbiohub#"/>
     <hyperlink ref="D18" r:id="rId6"/>
     <hyperlink ref="D2" r:id="rId7" display="http://sbols.org/v2#"/>
+    <hyperlink ref="D13" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId8"/>
+  <pageSetup orientation="landscape" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
@@ -27249,10 +27452,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB81"/>
+  <dimension ref="A1:AC81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -27268,11 +27471,11 @@
     <col min="9" max="9" width="10.15234375" customWidth="1"/>
     <col min="10" max="10" width="12.15234375" customWidth="1"/>
     <col min="11" max="11" width="9.921875" customWidth="1"/>
-    <col min="12" max="12" width="9.3046875" customWidth="1"/>
-    <col min="13" max="26" width="8.53515625" customWidth="1"/>
+    <col min="12" max="13" width="9.3046875" customWidth="1"/>
+    <col min="14" max="27" width="8.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -27287,7 +27490,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="M1" s="8"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -27301,8 +27504,9 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19"/>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -27317,7 +27521,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="M2" s="8"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -27331,8 +27535,9 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA2" s="1"/>
+    </row>
+    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -27345,9 +27550,10 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M3" s="8"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:29" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="37" t="s">
         <v>5</v>
       </c>
@@ -27361,7 +27567,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>7589</v>
+        <v>7588</v>
       </c>
       <c r="F4" s="39" t="s">
         <v>7575</v>
@@ -27370,7 +27576,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I4" s="40" t="s">
         <v>8</v>
@@ -27385,10 +27591,13 @@
         <v>11</v>
       </c>
       <c r="M4" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
         <v>14</v>
       </c>
@@ -27411,7 +27620,7 @@
         <v>7566</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I5" s="33" t="s">
         <v>16</v>
@@ -27425,12 +27634,15 @@
       <c r="L5" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="M5" s="30" t="str">
+      <c r="M5" s="56" t="s">
+        <v>7593</v>
+      </c>
+      <c r="N5" s="30" t="str">
         <f>Library!$I5&amp;":"&amp;Library!$J5</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="31" t="s">
         <v>7529</v>
       </c>
@@ -27453,7 +27665,7 @@
         <v>7567</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I6" s="33" t="s">
         <v>16</v>
@@ -27467,11 +27679,13 @@
       <c r="L6" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="M6" s="30" t="str">
+      <c r="M6" s="56" t="s">
+        <v>7594</v>
+      </c>
+      <c r="N6" s="30" t="str">
         <f>Library!$I6&amp;":"&amp;Library!$J6</f>
         <v>PubMed:28252958</v>
       </c>
-      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -27484,8 +27698,9 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC6" s="1"/>
+    </row>
+    <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>7530</v>
       </c>
@@ -27508,7 +27723,7 @@
         <v>7568</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I7" s="33" t="s">
         <v>16</v>
@@ -27522,11 +27737,13 @@
       <c r="L7" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="M7" s="30" t="str">
+      <c r="M7" s="56" t="s">
+        <v>7595</v>
+      </c>
+      <c r="N7" s="30" t="str">
         <f>Library!$I7&amp;":"&amp;Library!$J7</f>
         <v>PubMed:28252959</v>
       </c>
-      <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -27539,8 +27756,9 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC7" s="1"/>
+    </row>
+    <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
         <v>7531</v>
       </c>
@@ -27563,7 +27781,7 @@
         <v>7569</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I8" s="33" t="s">
         <v>16</v>
@@ -27577,11 +27795,13 @@
       <c r="L8" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="M8" s="30" t="str">
+      <c r="M8" s="56" t="s">
+        <v>7596</v>
+      </c>
+      <c r="N8" s="30" t="str">
         <f>Library!$I8&amp;":"&amp;Library!$J8</f>
         <v>PubMed:28252960</v>
       </c>
-      <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -27594,8 +27814,9 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC8" s="1"/>
+    </row>
+    <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="31" t="s">
         <v>7564</v>
       </c>
@@ -27616,7 +27837,7 @@
         <v>7572</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I9" s="33" t="s">
         <v>16</v>
@@ -27630,11 +27851,13 @@
       <c r="L9" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="M9" s="30" t="str">
+      <c r="M9" s="56" t="s">
+        <v>7593</v>
+      </c>
+      <c r="N9" s="30" t="str">
         <f>Library!$I9&amp;":"&amp;Library!$J9</f>
         <v>PubMed:28252961</v>
       </c>
-      <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -27647,8 +27870,9 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC9" s="1"/>
+    </row>
+    <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
         <v>7565</v>
       </c>
@@ -27669,7 +27893,7 @@
         <v>7565</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I10" s="33" t="s">
         <v>16</v>
@@ -27683,11 +27907,13 @@
       <c r="L10" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="M10" s="30" t="str">
+      <c r="M10" s="56" t="s">
+        <v>7593</v>
+      </c>
+      <c r="N10" s="30" t="str">
         <f>Library!$I10&amp;":"&amp;Library!$J10</f>
         <v>PubMed:28252962</v>
       </c>
-      <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -27700,8 +27926,9 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
         <v>7532</v>
       </c>
@@ -27724,7 +27951,7 @@
         <v>7570</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I11" s="33" t="s">
         <v>16</v>
@@ -27738,11 +27965,13 @@
       <c r="L11" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="M11" s="30" t="str">
+      <c r="M11" s="56" t="s">
+        <v>7593</v>
+      </c>
+      <c r="N11" s="30" t="str">
         <f>Library!$I11&amp;":"&amp;Library!$J11</f>
         <v>PubMed:28252963</v>
       </c>
-      <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -27755,8 +27984,9 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
         <v>7533</v>
       </c>
@@ -27779,7 +28009,7 @@
         <v>7571</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="I12" s="33" t="s">
         <v>16</v>
@@ -27793,11 +28023,13 @@
       <c r="L12" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="M12" s="30" t="str">
+      <c r="M12" s="56" t="s">
+        <v>7593</v>
+      </c>
+      <c r="N12" s="30" t="str">
         <f>Library!$I12&amp;":"&amp;Library!$J12</f>
         <v>PubMed:28252964</v>
       </c>
-      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -27810,72 +28042,72 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
-    </row>
-    <row r="24" spans="14:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="14:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N25" s="1"/>
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="24" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-    </row>
-    <row r="26" spans="14:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="O26" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="14:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="14:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="O28" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P28" s="1"/>
-    </row>
-    <row r="34" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="O35" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="34" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P35" s="1"/>
-    </row>
-    <row r="36" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N37" s="1"/>
+      <c r="Q35" s="1"/>
+    </row>
+    <row r="36" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
-    </row>
-    <row r="38" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="O38" s="1"/>
+      <c r="Q37" s="1"/>
+    </row>
+    <row r="38" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P38" s="1"/>
-    </row>
-    <row r="39" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N40" s="1"/>
+      <c r="Q38" s="1"/>
+    </row>
+    <row r="39" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O39" s="1"/>
+    </row>
+    <row r="40" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="O41" s="1"/>
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P41" s="1"/>
-    </row>
-    <row r="42" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N43" s="1"/>
+      <c r="Q41" s="1"/>
+    </row>
+    <row r="42" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
-    </row>
-    <row r="44" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="O44" s="1"/>
+      <c r="Q43" s="1"/>
+    </row>
+    <row r="44" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P44" s="1"/>
-    </row>
-    <row r="45" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="N45" s="1"/>
-      <c r="Q45" s="1"/>
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="O45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
@@ -27885,9 +28117,9 @@
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
-    </row>
-    <row r="46" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="O46" s="1"/>
+      <c r="AA45" s="1"/>
+    </row>
+    <row r="46" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -27899,9 +28131,9 @@
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
-    </row>
-    <row r="48" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q48" s="1"/>
+      <c r="AA46" s="1"/>
+    </row>
+    <row r="48" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
@@ -27911,24 +28143,24 @@
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
-    </row>
-    <row r="51" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="O52" s="1"/>
+      <c r="AA48" s="1"/>
+    </row>
+    <row r="51" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O51" s="1"/>
+    </row>
+    <row r="52" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P52" s="1"/>
-    </row>
-    <row r="53" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N54" s="1"/>
+      <c r="Q52" s="1"/>
+    </row>
+    <row r="53" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O53" s="1"/>
+    </row>
+    <row r="54" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
-    </row>
-    <row r="55" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="N55" s="1"/>
+      <c r="Q54" s="1"/>
+    </row>
+    <row r="55" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
@@ -27941,14 +28173,14 @@
       <c r="X55" s="1"/>
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
-    </row>
-    <row r="56" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N56" s="1"/>
+      <c r="AA55" s="1"/>
+    </row>
+    <row r="56" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
-    </row>
-    <row r="57" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="N57" s="1"/>
+      <c r="Q56" s="1"/>
+    </row>
+    <row r="57" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
@@ -27961,9 +28193,9 @@
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
-    </row>
-    <row r="58" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="O58" s="1"/>
+      <c r="AA57" s="1"/>
+    </row>
+    <row r="58" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
@@ -27975,12 +28207,12 @@
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
-    </row>
-    <row r="59" spans="14:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N59" s="1"/>
-    </row>
-    <row r="60" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="N60" s="1"/>
+      <c r="AA58" s="1"/>
+    </row>
+    <row r="59" spans="15:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
@@ -27993,9 +28225,9 @@
       <c r="X60" s="1"/>
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
-    </row>
-    <row r="61" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="O61" s="1"/>
+      <c r="AA60" s="1"/>
+    </row>
+    <row r="61" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -28007,9 +28239,9 @@
       <c r="X61" s="1"/>
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
-    </row>
-    <row r="63" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q63" s="1"/>
+      <c r="AA61" s="1"/>
+    </row>
+    <row r="63" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
@@ -28019,9 +28251,9 @@
       <c r="X63" s="1"/>
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
-    </row>
-    <row r="64" spans="14:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q64" s="1"/>
+      <c r="AA63" s="1"/>
+    </row>
+    <row r="64" spans="15:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
@@ -28031,9 +28263,9 @@
       <c r="X64" s="1"/>
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
-    </row>
-    <row r="66" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q66" s="1"/>
+      <c r="AA64" s="1"/>
+    </row>
+    <row r="66" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
@@ -28043,9 +28275,9 @@
       <c r="X66" s="1"/>
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
-    </row>
-    <row r="72" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q72" s="1"/>
+      <c r="AA66" s="1"/>
+    </row>
+    <row r="72" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
@@ -28055,9 +28287,9 @@
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
       <c r="Z72" s="1"/>
-    </row>
-    <row r="74" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q74" s="1"/>
+      <c r="AA72" s="1"/>
+    </row>
+    <row r="74" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
@@ -28067,9 +28299,9 @@
       <c r="X74" s="1"/>
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
-    </row>
-    <row r="75" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q75" s="1"/>
+      <c r="AA74" s="1"/>
+    </row>
+    <row r="75" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
@@ -28079,9 +28311,9 @@
       <c r="X75" s="1"/>
       <c r="Y75" s="1"/>
       <c r="Z75" s="1"/>
-    </row>
-    <row r="76" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q76" s="1"/>
+      <c r="AA75" s="1"/>
+    </row>
+    <row r="76" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
@@ -28091,9 +28323,9 @@
       <c r="X76" s="1"/>
       <c r="Y76" s="1"/>
       <c r="Z76" s="1"/>
-    </row>
-    <row r="77" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q77" s="1"/>
+      <c r="AA76" s="1"/>
+    </row>
+    <row r="77" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R77" s="1"/>
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
@@ -28103,9 +28335,9 @@
       <c r="X77" s="1"/>
       <c r="Y77" s="1"/>
       <c r="Z77" s="1"/>
-    </row>
-    <row r="78" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q78" s="1"/>
+      <c r="AA77" s="1"/>
+    </row>
+    <row r="78" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R78" s="1"/>
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
@@ -28115,9 +28347,9 @@
       <c r="X78" s="1"/>
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
-    </row>
-    <row r="80" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q80" s="1"/>
+      <c r="AA78" s="1"/>
+    </row>
+    <row r="80" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
@@ -28127,9 +28359,9 @@
       <c r="X80" s="1"/>
       <c r="Y80" s="1"/>
       <c r="Z80" s="1"/>
-    </row>
-    <row r="81" spans="17:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="Q81" s="1"/>
+      <c r="AA80" s="1"/>
+    </row>
+    <row r="81" spans="18:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
@@ -28139,12 +28371,16 @@
       <c r="X81" s="1"/>
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
+      <c r="AA81" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>